<commit_message>
rerun models and edit figures
time is now a factor in all models and made pairwise comparisons. remade rates figures and survival curve figures
</commit_message>
<xml_diff>
--- a/Growth/Output/Tables.xlsx
+++ b/Growth/Output/Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninahmunk/Desktop/Projects/Acropora_Regeneration-main/Growth/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FE173C-DCBA-B048-80FE-2186A5AEFBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477C8C04-7066-6140-B8E3-F03EE438C8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27220" windowHeight="16300" activeTab="3" xr2:uid="{93EC686E-7E07-024F-8313-03B2053EB837}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="8" xr2:uid="{93EC686E-7E07-024F-8313-03B2053EB837}"/>
   </bookViews>
   <sheets>
     <sheet name="growth.tables" sheetId="1" r:id="rId1"/>
@@ -487,8 +487,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -892,6 +892,49 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -939,49 +982,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3975,7 +3975,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13:Q19"/>
+      <selection activeCell="J9" sqref="J9:Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3987,40 +3987,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="J1" s="63" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="J1" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="10" t="s">
@@ -4199,42 +4199,42 @@
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="J9" s="67" t="s">
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="J9" s="82" t="s">
         <v>118</v>
       </c>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
-      <c r="O9" s="67"/>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="67"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="82"/>
+      <c r="O9" s="82"/>
+      <c r="P9" s="82"/>
+      <c r="Q9" s="82"/>
     </row>
     <row r="10" spans="1:17" ht="16" customHeight="1">
-      <c r="A10" s="64"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="67"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="67"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="82"/>
     </row>
     <row r="11" spans="1:17" ht="16" customHeight="1">
       <c r="A11" s="10" t="s">
@@ -4258,14 +4258,14 @@
       <c r="G11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="67"/>
-      <c r="O11" s="67"/>
-      <c r="P11" s="67"/>
-      <c r="Q11" s="67"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="82"/>
+      <c r="O11" s="82"/>
+      <c r="P11" s="82"/>
+      <c r="Q11" s="82"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="7" t="s">
@@ -4289,14 +4289,14 @@
       <c r="G12" s="7">
         <v>0.61599999999999999</v>
       </c>
-      <c r="J12" s="67"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="67"/>
-      <c r="P12" s="67"/>
-      <c r="Q12" s="67"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="82"/>
+      <c r="P12" s="82"/>
+      <c r="Q12" s="82"/>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="7" t="s">
@@ -4367,7 +4367,7 @@
       <c r="G14" s="7">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="J14" s="65" t="s">
+      <c r="J14" s="80" t="s">
         <v>112</v>
       </c>
       <c r="K14" s="44" t="s">
@@ -4393,7 +4393,7 @@
       </c>
     </row>
     <row r="15" spans="1:17">
-      <c r="J15" s="65"/>
+      <c r="J15" s="80"/>
       <c r="K15" s="44" t="s">
         <v>96</v>
       </c>
@@ -4417,7 +4417,7 @@
       </c>
     </row>
     <row r="16" spans="1:17">
-      <c r="J16" s="65"/>
+      <c r="J16" s="80"/>
       <c r="K16" s="42" t="s">
         <v>99</v>
       </c>
@@ -4441,7 +4441,7 @@
       </c>
     </row>
     <row r="17" spans="10:17">
-      <c r="J17" s="65" t="s">
+      <c r="J17" s="80" t="s">
         <v>130</v>
       </c>
       <c r="K17" s="44" t="s">
@@ -4467,7 +4467,7 @@
       </c>
     </row>
     <row r="18" spans="10:17">
-      <c r="J18" s="65"/>
+      <c r="J18" s="80"/>
       <c r="K18" s="44" t="s">
         <v>96</v>
       </c>
@@ -4491,7 +4491,7 @@
       </c>
     </row>
     <row r="19" spans="10:17">
-      <c r="J19" s="66"/>
+      <c r="J19" s="81"/>
       <c r="K19" s="48" t="s">
         <v>99</v>
       </c>
@@ -4537,7 +4537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557F2858-C4B9-7240-AE06-75EC26517FCF}">
   <dimension ref="H6:O69"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H6" sqref="H6:O65"/>
     </sheetView>
   </sheetViews>
@@ -4547,76 +4547,76 @@
   </cols>
   <sheetData>
     <row r="6" spans="8:15">
-      <c r="H6" s="67" t="s">
+      <c r="H6" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="67"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
     </row>
     <row r="7" spans="8:15">
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="67"/>
-      <c r="O7" s="67"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
     </row>
     <row r="8" spans="8:15">
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="67"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="82"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="82"/>
     </row>
     <row r="9" spans="8:15">
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
-      <c r="O9" s="67"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="82"/>
+      <c r="O9" s="82"/>
     </row>
     <row r="10" spans="8:15">
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="67"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="82"/>
     </row>
     <row r="11" spans="8:15">
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="67"/>
-      <c r="O11" s="67"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="82"/>
+      <c r="O11" s="82"/>
     </row>
     <row r="12" spans="8:15">
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="67"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="82"/>
     </row>
     <row r="13" spans="8:15">
       <c r="H13" s="47" t="s">
@@ -4645,7 +4645,7 @@
       </c>
     </row>
     <row r="14" spans="8:15">
-      <c r="H14" s="79" t="s">
+      <c r="H14" s="63" t="s">
         <v>35</v>
       </c>
       <c r="I14" s="55"/>
@@ -4953,7 +4953,7 @@
       </c>
     </row>
     <row r="27" spans="8:15">
-      <c r="H27" s="79" t="s">
+      <c r="H27" s="63" t="s">
         <v>104</v>
       </c>
       <c r="I27" s="44"/>
@@ -5084,7 +5084,7 @@
       <c r="N32" s="55">
         <v>12.084</v>
       </c>
-      <c r="O32" s="83">
+      <c r="O32" s="67">
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
@@ -5237,7 +5237,7 @@
       </c>
     </row>
     <row r="39" spans="8:15">
-      <c r="H39" s="80"/>
+      <c r="H39" s="64"/>
       <c r="I39" s="44" t="s">
         <v>99</v>
       </c>
@@ -5261,7 +5261,7 @@
       </c>
     </row>
     <row r="40" spans="8:15">
-      <c r="H40" s="79" t="s">
+      <c r="H40" s="63" t="s">
         <v>36</v>
       </c>
       <c r="I40" s="55"/>
@@ -5437,7 +5437,7 @@
       <c r="O50" s="60"/>
     </row>
     <row r="51" spans="8:15">
-      <c r="H51" s="80"/>
+      <c r="H51" s="64"/>
       <c r="I51" s="55" t="s">
         <v>96</v>
       </c>
@@ -5461,7 +5461,7 @@
       <c r="O52" s="60"/>
     </row>
     <row r="53" spans="8:15" ht="17">
-      <c r="H53" s="80" t="s">
+      <c r="H53" s="64" t="s">
         <v>56</v>
       </c>
       <c r="I53" s="55"/>
@@ -5546,7 +5546,7 @@
       <c r="L59" s="55"/>
       <c r="M59" s="55"/>
       <c r="N59" s="55"/>
-      <c r="O59" s="81"/>
+      <c r="O59" s="65"/>
     </row>
     <row r="60" spans="8:15">
       <c r="H60" s="42" t="s">
@@ -5560,7 +5560,7 @@
       <c r="L60" s="55"/>
       <c r="M60" s="55"/>
       <c r="N60" s="55"/>
-      <c r="O60" s="81"/>
+      <c r="O60" s="65"/>
     </row>
     <row r="61" spans="8:15">
       <c r="H61" s="42"/>
@@ -5572,7 +5572,7 @@
       <c r="L61" s="55"/>
       <c r="M61" s="55"/>
       <c r="N61" s="55"/>
-      <c r="O61" s="81"/>
+      <c r="O61" s="65"/>
     </row>
     <row r="62" spans="8:15">
       <c r="H62" s="42"/>
@@ -5584,7 +5584,7 @@
       <c r="L62" s="55"/>
       <c r="M62" s="55"/>
       <c r="N62" s="55"/>
-      <c r="O62" s="81"/>
+      <c r="O62" s="65"/>
     </row>
     <row r="63" spans="8:15">
       <c r="H63" s="42" t="s">
@@ -5598,7 +5598,7 @@
       <c r="L63" s="55"/>
       <c r="M63" s="55"/>
       <c r="N63" s="55"/>
-      <c r="O63" s="81"/>
+      <c r="O63" s="65"/>
     </row>
     <row r="64" spans="8:15">
       <c r="H64" s="61"/>
@@ -5610,7 +5610,7 @@
       <c r="L64" s="55"/>
       <c r="M64" s="55"/>
       <c r="N64" s="55"/>
-      <c r="O64" s="81"/>
+      <c r="O64" s="65"/>
     </row>
     <row r="65" spans="8:15">
       <c r="H65" s="61"/>
@@ -5622,7 +5622,7 @@
       <c r="L65" s="55"/>
       <c r="M65" s="55"/>
       <c r="N65" s="55"/>
-      <c r="O65" s="81"/>
+      <c r="O65" s="65"/>
     </row>
     <row r="66" spans="8:15">
       <c r="H66" s="61"/>
@@ -5632,7 +5632,7 @@
       <c r="L66" s="55"/>
       <c r="M66" s="55"/>
       <c r="N66" s="55"/>
-      <c r="O66" s="81"/>
+      <c r="O66" s="65"/>
     </row>
     <row r="67" spans="8:15">
       <c r="H67" s="61"/>
@@ -5642,7 +5642,7 @@
       <c r="L67" s="55"/>
       <c r="M67" s="55"/>
       <c r="N67" s="55"/>
-      <c r="O67" s="81"/>
+      <c r="O67" s="65"/>
     </row>
     <row r="68" spans="8:15">
       <c r="H68" s="61"/>
@@ -5652,7 +5652,7 @@
       <c r="L68" s="55"/>
       <c r="M68" s="55"/>
       <c r="N68" s="55"/>
-      <c r="O68" s="81"/>
+      <c r="O68" s="65"/>
     </row>
     <row r="69" spans="8:15">
       <c r="H69" s="61"/>
@@ -5662,7 +5662,7 @@
       <c r="L69" s="55"/>
       <c r="M69" s="55"/>
       <c r="N69" s="55"/>
-      <c r="O69" s="81"/>
+      <c r="O69" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5683,7 +5683,7 @@
   </sheetPr>
   <dimension ref="D5:K68"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A56" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:K11"/>
     </sheetView>
   </sheetViews>
@@ -5697,76 +5697,76 @@
   </cols>
   <sheetData>
     <row r="5" spans="4:11">
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
     </row>
     <row r="6" spans="4:11">
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
     </row>
     <row r="7" spans="4:11">
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="93"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
     </row>
     <row r="8" spans="4:11">
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
     </row>
     <row r="9" spans="4:11">
-      <c r="D9" s="67" t="s">
+      <c r="D9" s="82" t="s">
         <v>127</v>
       </c>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="82"/>
     </row>
     <row r="10" spans="4:11">
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
     </row>
     <row r="11" spans="4:11">
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
     </row>
     <row r="12" spans="4:11">
       <c r="D12" s="47" t="s">
@@ -5795,7 +5795,7 @@
       </c>
     </row>
     <row r="13" spans="4:11">
-      <c r="D13" s="79" t="s">
+      <c r="D13" s="63" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="55"/>
@@ -5813,13 +5813,13 @@
       <c r="E14" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F14" s="82">
+      <c r="F14" s="66">
         <v>2.3473000000000001E-2</v>
       </c>
-      <c r="G14" s="82">
+      <c r="G14" s="66">
         <v>1.1736999999999999E-2</v>
       </c>
-      <c r="H14" s="91">
+      <c r="H14" s="75">
         <v>2</v>
       </c>
       <c r="I14" s="59">
@@ -5837,13 +5837,13 @@
       <c r="E15" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F15" s="82">
+      <c r="F15" s="66">
         <v>2.2866000000000001E-2</v>
       </c>
-      <c r="G15" s="82">
+      <c r="G15" s="66">
         <v>2.2866000000000001E-2</v>
       </c>
-      <c r="H15" s="91">
+      <c r="H15" s="75">
         <v>1</v>
       </c>
       <c r="I15" s="59">
@@ -5861,13 +5861,13 @@
       <c r="E16" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F16" s="82">
+      <c r="F16" s="66">
         <v>2.1946E-2</v>
       </c>
-      <c r="G16" s="82">
+      <c r="G16" s="66">
         <v>1.0973E-2</v>
       </c>
-      <c r="H16" s="91">
+      <c r="H16" s="75">
         <v>2</v>
       </c>
       <c r="I16" s="59">
@@ -5887,13 +5887,13 @@
       <c r="E17" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F17" s="82">
+      <c r="F17" s="66">
         <v>8.3476999999999996E-3</v>
       </c>
-      <c r="G17" s="82">
+      <c r="G17" s="66">
         <v>4.1739000000000004E-3</v>
       </c>
-      <c r="H17" s="92">
+      <c r="H17" s="76">
         <v>2</v>
       </c>
       <c r="I17" s="59">
@@ -5911,13 +5911,13 @@
       <c r="E18" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="82">
+      <c r="F18" s="66">
         <v>1.5220000000000001E-4</v>
       </c>
-      <c r="G18" s="82">
+      <c r="G18" s="66">
         <v>1.5220000000000001E-4</v>
       </c>
-      <c r="H18" s="91">
+      <c r="H18" s="75">
         <v>1</v>
       </c>
       <c r="I18" s="59">
@@ -5935,13 +5935,13 @@
       <c r="E19" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="82">
+      <c r="F19" s="66">
         <v>8.7086000000000004E-3</v>
       </c>
-      <c r="G19" s="82">
+      <c r="G19" s="66">
         <v>4.3543000000000002E-3</v>
       </c>
-      <c r="H19" s="91">
+      <c r="H19" s="75">
         <v>2</v>
       </c>
       <c r="I19" s="59">
@@ -5961,13 +5961,13 @@
       <c r="E20" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="82">
+      <c r="F20" s="66">
         <v>1.7772E-2</v>
       </c>
-      <c r="G20" s="82">
+      <c r="G20" s="66">
         <v>8.8859999999999998E-3</v>
       </c>
-      <c r="H20" s="91">
+      <c r="H20" s="75">
         <v>2</v>
       </c>
       <c r="I20" s="59">
@@ -5985,13 +5985,13 @@
       <c r="E21" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F21" s="82">
+      <c r="F21" s="66">
         <v>0.230213</v>
       </c>
-      <c r="G21" s="82">
+      <c r="G21" s="66">
         <v>0.230213</v>
       </c>
-      <c r="H21" s="91">
+      <c r="H21" s="75">
         <v>1</v>
       </c>
       <c r="I21" s="59">
@@ -6000,7 +6000,7 @@
       <c r="J21" s="59">
         <v>20.9847</v>
       </c>
-      <c r="K21" s="83" t="s">
+      <c r="K21" s="67" t="s">
         <v>128</v>
       </c>
     </row>
@@ -6009,13 +6009,13 @@
       <c r="E22" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F22" s="82">
+      <c r="F22" s="66">
         <v>2.65E-3</v>
       </c>
-      <c r="G22" s="82">
+      <c r="G22" s="66">
         <v>1.325E-3</v>
       </c>
-      <c r="H22" s="91">
+      <c r="H22" s="75">
         <v>2</v>
       </c>
       <c r="I22" s="59">
@@ -6035,22 +6035,22 @@
       <c r="E23" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F23" s="86">
+      <c r="F23" s="70">
         <v>1.9227999999999999E-2</v>
       </c>
-      <c r="G23" s="86">
+      <c r="G23" s="70">
         <v>9.6139999999999993E-3</v>
       </c>
-      <c r="H23" s="91">
-        <v>2</v>
-      </c>
-      <c r="I23" s="89">
+      <c r="H23" s="75">
+        <v>2</v>
+      </c>
+      <c r="I23" s="73">
         <v>60.938000000000002</v>
       </c>
-      <c r="J23" s="89">
+      <c r="J23" s="73">
         <v>0.98319999999999996</v>
       </c>
-      <c r="K23" s="89">
+      <c r="K23" s="73">
         <v>0.37997399999999998</v>
       </c>
     </row>
@@ -6059,22 +6059,22 @@
       <c r="E24" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F24" s="86">
+      <c r="F24" s="70">
         <v>0.111959</v>
       </c>
-      <c r="G24" s="86">
+      <c r="G24" s="70">
         <v>0.111959</v>
       </c>
-      <c r="H24" s="91">
-        <v>1</v>
-      </c>
-      <c r="I24" s="89">
+      <c r="H24" s="75">
+        <v>1</v>
+      </c>
+      <c r="I24" s="73">
         <v>60.914000000000001</v>
       </c>
-      <c r="J24" s="89">
+      <c r="J24" s="73">
         <v>11.4496</v>
       </c>
-      <c r="K24" s="88">
+      <c r="K24" s="72">
         <v>1.255E-3</v>
       </c>
     </row>
@@ -6083,36 +6083,36 @@
       <c r="E25" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F25" s="86">
+      <c r="F25" s="70">
         <v>0.13087799999999999</v>
       </c>
-      <c r="G25" s="86">
+      <c r="G25" s="70">
         <v>6.5438999999999997E-2</v>
       </c>
-      <c r="H25" s="91">
-        <v>2</v>
-      </c>
-      <c r="I25" s="89">
+      <c r="H25" s="75">
+        <v>2</v>
+      </c>
+      <c r="I25" s="73">
         <v>61.021000000000001</v>
       </c>
-      <c r="J25" s="89">
+      <c r="J25" s="73">
         <v>6.6921999999999997</v>
       </c>
-      <c r="K25" s="88">
+      <c r="K25" s="72">
         <v>2.3570000000000002E-3</v>
       </c>
     </row>
     <row r="26" spans="4:11">
-      <c r="D26" s="79" t="s">
+      <c r="D26" s="63" t="s">
         <v>104</v>
       </c>
       <c r="E26" s="44"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="92"/>
-      <c r="I26" s="89"/>
-      <c r="J26" s="89"/>
-      <c r="K26" s="89"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="73"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="73"/>
     </row>
     <row r="27" spans="4:11" ht="17">
       <c r="D27" s="61" t="s">
@@ -6121,13 +6121,13 @@
       <c r="E27" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="82">
+      <c r="F27" s="66">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="G27" s="82">
+      <c r="G27" s="66">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="H27" s="91">
+      <c r="H27" s="75">
         <v>2</v>
       </c>
       <c r="I27" s="59">
@@ -6136,7 +6136,7 @@
       <c r="J27" s="59">
         <v>0.1113</v>
       </c>
-      <c r="K27" s="89">
+      <c r="K27" s="73">
         <v>0.89480000000000004</v>
       </c>
     </row>
@@ -6145,13 +6145,13 @@
       <c r="E28" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F28" s="82">
+      <c r="F28" s="66">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G28" s="82">
+      <c r="G28" s="66">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="H28" s="91">
+      <c r="H28" s="75">
         <v>1</v>
       </c>
       <c r="I28" s="59">
@@ -6160,7 +6160,7 @@
       <c r="J28" s="59">
         <v>0.13389999999999999</v>
       </c>
-      <c r="K28" s="89">
+      <c r="K28" s="73">
         <v>0.7157</v>
       </c>
     </row>
@@ -6169,13 +6169,13 @@
       <c r="E29" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F29" s="82">
+      <c r="F29" s="66">
         <v>7.4000000000000003E-3</v>
       </c>
-      <c r="G29" s="82">
+      <c r="G29" s="66">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="H29" s="91">
+      <c r="H29" s="75">
         <v>2</v>
       </c>
       <c r="I29" s="59">
@@ -6184,7 +6184,7 @@
       <c r="J29" s="59">
         <v>1.0548</v>
       </c>
-      <c r="K29" s="89">
+      <c r="K29" s="73">
         <v>0.35449999999999998</v>
       </c>
     </row>
@@ -6195,22 +6195,22 @@
       <c r="E30" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F30" s="86">
+      <c r="F30" s="70">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="G30" s="86">
+      <c r="G30" s="70">
         <v>1.8E-3</v>
       </c>
-      <c r="H30" s="92">
-        <v>2</v>
-      </c>
-      <c r="I30" s="89">
+      <c r="H30" s="76">
+        <v>2</v>
+      </c>
+      <c r="I30" s="73">
         <v>61.530999999999999</v>
       </c>
-      <c r="J30" s="89">
+      <c r="J30" s="73">
         <v>0.66510000000000002</v>
       </c>
-      <c r="K30" s="89">
+      <c r="K30" s="73">
         <v>0.51790000000000003</v>
       </c>
     </row>
@@ -6219,13 +6219,13 @@
       <c r="E31" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="82">
+      <c r="F31" s="66">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="G31" s="82">
+      <c r="G31" s="66">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="H31" s="91">
+      <c r="H31" s="75">
         <v>1</v>
       </c>
       <c r="I31" s="59">
@@ -6234,7 +6234,7 @@
       <c r="J31" s="59">
         <v>12.084</v>
       </c>
-      <c r="K31" s="87" t="s">
+      <c r="K31" s="71" t="s">
         <v>129</v>
       </c>
     </row>
@@ -6243,13 +6243,13 @@
       <c r="E32" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F32" s="82">
+      <c r="F32" s="66">
         <v>4.7000000000000002E-3</v>
       </c>
-      <c r="G32" s="82">
+      <c r="G32" s="66">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="H32" s="91">
+      <c r="H32" s="75">
         <v>2</v>
       </c>
       <c r="I32" s="59">
@@ -6269,13 +6269,13 @@
       <c r="E33" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F33" s="82">
+      <c r="F33" s="66">
         <v>1.45548E-2</v>
       </c>
-      <c r="G33" s="82">
+      <c r="G33" s="66">
         <v>7.2773999999999998E-3</v>
       </c>
-      <c r="H33" s="91">
+      <c r="H33" s="75">
         <v>2</v>
       </c>
       <c r="I33" s="59">
@@ -6293,13 +6293,13 @@
       <c r="E34" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F34" s="82">
+      <c r="F34" s="66">
         <v>7.7629999999999995E-4</v>
       </c>
-      <c r="G34" s="82">
+      <c r="G34" s="66">
         <v>7.7629999999999995E-4</v>
       </c>
-      <c r="H34" s="91">
+      <c r="H34" s="75">
         <v>1</v>
       </c>
       <c r="I34" s="59">
@@ -6317,13 +6317,13 @@
       <c r="E35" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F35" s="82">
+      <c r="F35" s="66">
         <v>7.4022000000000003E-3</v>
       </c>
-      <c r="G35" s="82">
+      <c r="G35" s="66">
         <v>3.7011000000000001E-3</v>
       </c>
-      <c r="H35" s="91">
+      <c r="H35" s="75">
         <v>2</v>
       </c>
       <c r="I35" s="59">
@@ -6343,13 +6343,13 @@
       <c r="E36" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="82">
+      <c r="F36" s="66">
         <v>1.45548E-2</v>
       </c>
-      <c r="G36" s="82">
+      <c r="G36" s="66">
         <v>7.2773999999999998E-3</v>
       </c>
-      <c r="H36" s="91">
+      <c r="H36" s="75">
         <v>2</v>
       </c>
       <c r="I36" s="59">
@@ -6367,13 +6367,13 @@
       <c r="E37" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F37" s="82">
+      <c r="F37" s="66">
         <v>7.7629999999999995E-4</v>
       </c>
-      <c r="G37" s="82">
+      <c r="G37" s="66">
         <v>7.7629999999999995E-4</v>
       </c>
-      <c r="H37" s="91">
+      <c r="H37" s="75">
         <v>1</v>
       </c>
       <c r="I37" s="59">
@@ -6387,17 +6387,17 @@
       </c>
     </row>
     <row r="38" spans="4:11">
-      <c r="D38" s="80"/>
+      <c r="D38" s="64"/>
       <c r="E38" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F38" s="82">
+      <c r="F38" s="66">
         <v>7.4022000000000003E-3</v>
       </c>
-      <c r="G38" s="82">
+      <c r="G38" s="66">
         <v>3.7011000000000001E-3</v>
       </c>
-      <c r="H38" s="91">
+      <c r="H38" s="75">
         <v>2</v>
       </c>
       <c r="I38" s="59">
@@ -6411,13 +6411,13 @@
       </c>
     </row>
     <row r="39" spans="4:11">
-      <c r="D39" s="79" t="s">
+      <c r="D39" s="63" t="s">
         <v>36</v>
       </c>
       <c r="E39" s="55"/>
-      <c r="F39" s="82"/>
-      <c r="G39" s="82"/>
-      <c r="H39" s="91"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="75"/>
       <c r="I39" s="59"/>
       <c r="J39" s="59"/>
       <c r="K39" s="59"/>
@@ -6429,13 +6429,13 @@
       <c r="E40" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F40" s="82">
+      <c r="F40" s="66">
         <v>3.3536000000000003E-2</v>
       </c>
-      <c r="G40" s="82">
+      <c r="G40" s="66">
         <v>1.6768000000000002E-2</v>
       </c>
-      <c r="H40" s="91">
+      <c r="H40" s="75">
         <v>2</v>
       </c>
       <c r="I40" s="59">
@@ -6453,13 +6453,13 @@
       <c r="E41" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F41" s="82">
+      <c r="F41" s="66">
         <v>3.0291999999999999E-2</v>
       </c>
-      <c r="G41" s="82">
+      <c r="G41" s="66">
         <v>3.0291999999999999E-2</v>
       </c>
-      <c r="H41" s="91">
+      <c r="H41" s="75">
         <v>1</v>
       </c>
       <c r="I41" s="59">
@@ -6477,13 +6477,13 @@
       <c r="E42" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F42" s="82">
+      <c r="F42" s="66">
         <v>5.4202E-2</v>
       </c>
-      <c r="G42" s="82">
+      <c r="G42" s="66">
         <v>2.7101E-2</v>
       </c>
-      <c r="H42" s="91">
+      <c r="H42" s="75">
         <v>2</v>
       </c>
       <c r="I42" s="59">
@@ -6497,16 +6497,16 @@
       </c>
     </row>
     <row r="43" spans="4:11" ht="17">
-      <c r="D43" s="80" t="s">
+      <c r="D43" s="64" t="s">
         <v>56</v>
       </c>
       <c r="E43" s="55"/>
-      <c r="F43" s="82"/>
-      <c r="G43" s="82"/>
-      <c r="H43" s="91"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="75"/>
       <c r="I43" s="59"/>
       <c r="J43" s="59"/>
-      <c r="K43" s="89"/>
+      <c r="K43" s="73"/>
     </row>
     <row r="44" spans="4:11" ht="17">
       <c r="D44" s="61" t="s">
@@ -6515,13 +6515,13 @@
       <c r="E44" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="82">
+      <c r="F44" s="66">
         <v>2.3921000000000001E-2</v>
       </c>
-      <c r="G44" s="82">
+      <c r="G44" s="66">
         <v>1.19604E-2</v>
       </c>
-      <c r="H44" s="91">
+      <c r="H44" s="75">
         <v>2</v>
       </c>
       <c r="I44" s="59">
@@ -6530,7 +6530,7 @@
       <c r="J44" s="59">
         <v>0.97050000000000003</v>
       </c>
-      <c r="K44" s="89">
+      <c r="K44" s="73">
         <v>0.3846</v>
       </c>
     </row>
@@ -6539,13 +6539,13 @@
       <c r="E45" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F45" s="82">
+      <c r="F45" s="66">
         <v>2.8018999999999999E-2</v>
       </c>
-      <c r="G45" s="82">
+      <c r="G45" s="66">
         <v>2.8018700000000001E-2</v>
       </c>
-      <c r="H45" s="91">
+      <c r="H45" s="75">
         <v>1</v>
       </c>
       <c r="I45" s="59">
@@ -6554,7 +6554,7 @@
       <c r="J45" s="59">
         <v>2.2734999999999999</v>
       </c>
-      <c r="K45" s="89">
+      <c r="K45" s="73">
         <v>0.13669999999999999</v>
       </c>
     </row>
@@ -6563,13 +6563,13 @@
       <c r="E46" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F46" s="82">
+      <c r="F46" s="66">
         <v>1.4961E-2</v>
       </c>
-      <c r="G46" s="82">
+      <c r="G46" s="66">
         <v>7.4806999999999998E-3</v>
       </c>
-      <c r="H46" s="91">
+      <c r="H46" s="75">
         <v>2</v>
       </c>
       <c r="I46" s="59">
@@ -6578,7 +6578,7 @@
       <c r="J46" s="59">
         <v>0.60699999999999998</v>
       </c>
-      <c r="K46" s="89">
+      <c r="K46" s="73">
         <v>0.54820000000000002</v>
       </c>
     </row>
@@ -6589,13 +6589,13 @@
       <c r="E47" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="82">
+      <c r="F47" s="66">
         <v>5.2700999999999998E-3</v>
       </c>
-      <c r="G47" s="82">
+      <c r="G47" s="66">
         <v>2.6351E-3</v>
       </c>
-      <c r="H47" s="92">
+      <c r="H47" s="76">
         <v>2</v>
       </c>
       <c r="I47" s="59">
@@ -6604,7 +6604,7 @@
       <c r="J47" s="59">
         <v>0.14330000000000001</v>
       </c>
-      <c r="K47" s="89">
+      <c r="K47" s="73">
         <v>0.86670000000000003</v>
       </c>
     </row>
@@ -6613,13 +6613,13 @@
       <c r="E48" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F48" s="82">
+      <c r="F48" s="66">
         <v>2.79014E-2</v>
       </c>
-      <c r="G48" s="82">
+      <c r="G48" s="66">
         <v>2.79014E-2</v>
       </c>
-      <c r="H48" s="91">
+      <c r="H48" s="75">
         <v>1</v>
       </c>
       <c r="I48" s="59">
@@ -6628,7 +6628,7 @@
       <c r="J48" s="59">
         <v>1.5178</v>
       </c>
-      <c r="K48" s="89">
+      <c r="K48" s="73">
         <v>0.22259999999999999</v>
       </c>
     </row>
@@ -6637,13 +6637,13 @@
       <c r="E49" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F49" s="82">
+      <c r="F49" s="66">
         <v>1.2933E-3</v>
       </c>
-      <c r="G49" s="82">
+      <c r="G49" s="66">
         <v>6.4670000000000005E-4</v>
       </c>
-      <c r="H49" s="91">
+      <c r="H49" s="75">
         <v>2</v>
       </c>
       <c r="I49" s="59">
@@ -6652,7 +6652,7 @@
       <c r="J49" s="59">
         <v>3.5200000000000002E-2</v>
       </c>
-      <c r="K49" s="89">
+      <c r="K49" s="73">
         <v>0.96550000000000002</v>
       </c>
     </row>
@@ -6663,13 +6663,13 @@
       <c r="E50" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F50" s="82">
+      <c r="F50" s="66">
         <v>2.9399999999999999E-3</v>
       </c>
-      <c r="G50" s="82">
+      <c r="G50" s="66">
         <v>1.47E-3</v>
       </c>
-      <c r="H50" s="91">
+      <c r="H50" s="75">
         <v>2</v>
       </c>
       <c r="I50" s="59">
@@ -6678,7 +6678,7 @@
       <c r="J50" s="59">
         <v>7.3700000000000002E-2</v>
       </c>
-      <c r="K50" s="89">
+      <c r="K50" s="73">
         <v>0.92904089999999995</v>
       </c>
     </row>
@@ -6687,13 +6687,13 @@
       <c r="E51" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F51" s="82">
+      <c r="F51" s="66">
         <v>0.3301</v>
       </c>
-      <c r="G51" s="82">
+      <c r="G51" s="66">
         <v>0.3301</v>
       </c>
-      <c r="H51" s="91">
+      <c r="H51" s="75">
         <v>1</v>
       </c>
       <c r="I51" s="59">
@@ -6702,7 +6702,7 @@
       <c r="J51" s="59">
         <v>16.560199999999998</v>
       </c>
-      <c r="K51" s="88" t="s">
+      <c r="K51" s="72" t="s">
         <v>129</v>
       </c>
     </row>
@@ -6711,13 +6711,13 @@
       <c r="E52" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F52" s="82">
+      <c r="F52" s="66">
         <v>2.97E-3</v>
       </c>
-      <c r="G52" s="82">
+      <c r="G52" s="66">
         <v>1.48E-3</v>
       </c>
-      <c r="H52" s="91">
+      <c r="H52" s="75">
         <v>2</v>
       </c>
       <c r="I52" s="59">
@@ -6726,7 +6726,7 @@
       <c r="J52" s="59">
         <v>7.4399999999999994E-2</v>
       </c>
-      <c r="K52" s="89">
+      <c r="K52" s="73">
         <v>0.92838410000000005</v>
       </c>
     </row>
@@ -6737,13 +6737,13 @@
       <c r="E53" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F53" s="82">
+      <c r="F53" s="66">
         <v>1.2383999999999999E-2</v>
       </c>
-      <c r="G53" s="82">
+      <c r="G53" s="66">
         <v>6.1919999999999996E-3</v>
       </c>
-      <c r="H53" s="91">
+      <c r="H53" s="75">
         <v>2</v>
       </c>
       <c r="I53" s="59">
@@ -6752,7 +6752,7 @@
       <c r="J53" s="59">
         <v>0.53749999999999998</v>
       </c>
-      <c r="K53" s="89">
+      <c r="K53" s="73">
         <v>0.58695090000000005</v>
       </c>
     </row>
@@ -6761,13 +6761,13 @@
       <c r="E54" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F54" s="82">
+      <c r="F54" s="66">
         <v>0.17271600000000001</v>
       </c>
-      <c r="G54" s="82">
+      <c r="G54" s="66">
         <v>0.17271600000000001</v>
       </c>
-      <c r="H54" s="91">
+      <c r="H54" s="75">
         <v>1</v>
       </c>
       <c r="I54" s="59">
@@ -6776,7 +6776,7 @@
       <c r="J54" s="59">
         <v>14.991400000000001</v>
       </c>
-      <c r="K54" s="88" t="s">
+      <c r="K54" s="72" t="s">
         <v>129</v>
       </c>
     </row>
@@ -6785,13 +6785,13 @@
       <c r="E55" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F55" s="82">
+      <c r="F55" s="66">
         <v>0.15382499999999999</v>
       </c>
-      <c r="G55" s="82">
+      <c r="G55" s="66">
         <v>7.6911999999999994E-2</v>
       </c>
-      <c r="H55" s="91">
+      <c r="H55" s="75">
         <v>2</v>
       </c>
       <c r="I55" s="59">
@@ -6800,21 +6800,21 @@
       <c r="J55" s="59">
         <v>6.6757999999999997</v>
       </c>
-      <c r="K55" s="88">
+      <c r="K55" s="72">
         <v>2.3776000000000001E-3</v>
       </c>
     </row>
     <row r="56" spans="4:11" ht="17">
-      <c r="D56" s="84" t="s">
+      <c r="D56" s="68" t="s">
         <v>58</v>
       </c>
       <c r="E56" s="55"/>
-      <c r="F56" s="82"/>
-      <c r="G56" s="82"/>
-      <c r="H56" s="91"/>
+      <c r="F56" s="66"/>
+      <c r="G56" s="66"/>
+      <c r="H56" s="75"/>
       <c r="I56" s="59"/>
       <c r="J56" s="59"/>
-      <c r="K56" s="90"/>
+      <c r="K56" s="74"/>
     </row>
     <row r="57" spans="4:11" ht="17">
       <c r="D57" s="61" t="s">
@@ -6823,13 +6823,13 @@
       <c r="E57" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F57" s="82">
+      <c r="F57" s="66">
         <v>90.97</v>
       </c>
-      <c r="G57" s="82">
+      <c r="G57" s="66">
         <v>45.48</v>
       </c>
-      <c r="H57" s="91">
+      <c r="H57" s="75">
         <v>2</v>
       </c>
       <c r="I57" s="59">
@@ -6838,7 +6838,7 @@
       <c r="J57" s="59">
         <v>0.53239999999999998</v>
       </c>
-      <c r="K57" s="89">
+      <c r="K57" s="73">
         <v>0.59030000000000005</v>
       </c>
     </row>
@@ -6847,13 +6847,13 @@
       <c r="E58" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F58" s="82">
+      <c r="F58" s="66">
         <v>444.12</v>
       </c>
-      <c r="G58" s="82">
+      <c r="G58" s="66">
         <v>444.12</v>
       </c>
-      <c r="H58" s="91">
+      <c r="H58" s="75">
         <v>1</v>
       </c>
       <c r="I58" s="59">
@@ -6862,7 +6862,7 @@
       <c r="J58" s="59">
         <v>5.1984000000000004</v>
       </c>
-      <c r="K58" s="90">
+      <c r="K58" s="74">
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
@@ -6871,13 +6871,13 @@
       <c r="E59" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F59" s="82">
+      <c r="F59" s="66">
         <v>134</v>
       </c>
-      <c r="G59" s="82">
+      <c r="G59" s="66">
         <v>67</v>
       </c>
-      <c r="H59" s="91">
+      <c r="H59" s="75">
         <v>2</v>
       </c>
       <c r="I59" s="59">
@@ -6886,7 +6886,7 @@
       <c r="J59" s="59">
         <v>0.78420000000000001</v>
       </c>
-      <c r="K59" s="89">
+      <c r="K59" s="73">
         <v>0.46160000000000001</v>
       </c>
     </row>
@@ -6897,13 +6897,13 @@
       <c r="E60" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F60" s="82">
+      <c r="F60" s="66">
         <v>285.67</v>
       </c>
-      <c r="G60" s="82">
+      <c r="G60" s="66">
         <v>142.834</v>
       </c>
-      <c r="H60" s="92">
+      <c r="H60" s="76">
         <v>2</v>
       </c>
       <c r="I60" s="59">
@@ -6912,7 +6912,7 @@
       <c r="J60" s="59">
         <v>0.5696</v>
       </c>
-      <c r="K60" s="89">
+      <c r="K60" s="73">
         <v>0.56869999999999998</v>
       </c>
     </row>
@@ -6921,13 +6921,13 @@
       <c r="E61" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F61" s="82">
+      <c r="F61" s="66">
         <v>0.5</v>
       </c>
-      <c r="G61" s="82">
+      <c r="G61" s="66">
         <v>0.497</v>
       </c>
-      <c r="H61" s="91">
+      <c r="H61" s="75">
         <v>1</v>
       </c>
       <c r="I61" s="59">
@@ -6936,7 +6936,7 @@
       <c r="J61" s="59">
         <v>2E-3</v>
       </c>
-      <c r="K61" s="89">
+      <c r="K61" s="73">
         <v>0.9647</v>
       </c>
     </row>
@@ -6945,13 +6945,13 @@
       <c r="E62" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F62" s="82">
+      <c r="F62" s="66">
         <v>452.02</v>
       </c>
-      <c r="G62" s="82">
+      <c r="G62" s="66">
         <v>226.00899999999999</v>
       </c>
-      <c r="H62" s="91">
+      <c r="H62" s="75">
         <v>2</v>
       </c>
       <c r="I62" s="59">
@@ -6960,7 +6960,7 @@
       <c r="J62" s="59">
         <v>0.9012</v>
       </c>
-      <c r="K62" s="89">
+      <c r="K62" s="73">
         <v>0.4113</v>
       </c>
     </row>
@@ -6971,13 +6971,13 @@
       <c r="E63" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F63" s="82">
+      <c r="F63" s="66">
         <v>35.549999999999997</v>
       </c>
-      <c r="G63" s="82">
+      <c r="G63" s="66">
         <v>17.77</v>
       </c>
-      <c r="H63" s="91">
+      <c r="H63" s="75">
         <v>2</v>
       </c>
       <c r="I63" s="59">
@@ -6986,7 +6986,7 @@
       <c r="J63" s="59">
         <v>8.8400000000000006E-2</v>
       </c>
-      <c r="K63" s="89">
+      <c r="K63" s="73">
         <v>0.91552540000000004</v>
       </c>
     </row>
@@ -6995,13 +6995,13 @@
       <c r="E64" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="F64" s="82">
+      <c r="F64" s="66">
         <v>35.549999999999997</v>
       </c>
-      <c r="G64" s="82">
+      <c r="G64" s="66">
         <v>2701.15</v>
       </c>
-      <c r="H64" s="91">
+      <c r="H64" s="75">
         <v>1</v>
       </c>
       <c r="I64" s="59">
@@ -7010,7 +7010,7 @@
       <c r="J64" s="59">
         <v>13.4329</v>
       </c>
-      <c r="K64" s="85" t="s">
+      <c r="K64" s="69" t="s">
         <v>129</v>
       </c>
     </row>
@@ -7019,13 +7019,13 @@
       <c r="E65" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F65" s="82">
+      <c r="F65" s="66">
         <v>1307.07</v>
       </c>
-      <c r="G65" s="82">
+      <c r="G65" s="66">
         <v>653.53</v>
       </c>
-      <c r="H65" s="91">
+      <c r="H65" s="75">
         <v>2</v>
       </c>
       <c r="I65" s="59">
@@ -7034,7 +7034,7 @@
       <c r="J65" s="59">
         <v>3.2501000000000002</v>
       </c>
-      <c r="K65" s="88">
+      <c r="K65" s="72">
         <v>4.5490700000000002E-2</v>
       </c>
     </row>
@@ -7046,7 +7046,7 @@
       <c r="H66" s="55"/>
       <c r="I66" s="55"/>
       <c r="J66" s="55"/>
-      <c r="K66" s="81"/>
+      <c r="K66" s="65"/>
     </row>
     <row r="67" spans="4:11">
       <c r="D67" s="61"/>
@@ -7056,7 +7056,7 @@
       <c r="H67" s="55"/>
       <c r="I67" s="55"/>
       <c r="J67" s="55"/>
-      <c r="K67" s="81"/>
+      <c r="K67" s="65"/>
     </row>
     <row r="68" spans="4:11">
       <c r="D68" s="61"/>
@@ -7066,7 +7066,7 @@
       <c r="H68" s="55"/>
       <c r="I68" s="55"/>
       <c r="J68" s="55"/>
-      <c r="K68" s="81"/>
+      <c r="K68" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7087,8 +7087,8 @@
   </sheetPr>
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7105,41 +7105,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="I1" s="67" t="s">
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="I1" s="82" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
     </row>
     <row r="2" spans="1:13" ht="16" customHeight="1">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
+      <c r="A2" s="84"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="70"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
+      <c r="A3" s="85"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
@@ -7154,11 +7154,11 @@
       <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="33" t="s">
@@ -7167,11 +7167,11 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="67"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="5" t="s">
@@ -7184,11 +7184,11 @@
         <v>17</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="5" t="s">
@@ -7203,11 +7203,11 @@
       <c r="D7" s="1">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="67"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="33" t="s">
@@ -7361,12 +7361,12 @@
       <c r="M14" s="49"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="83" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
       <c r="I15" s="42"/>
       <c r="J15" s="42" t="s">
         <v>110</v>
@@ -7382,10 +7382,10 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="69"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
+      <c r="A16" s="84"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="84"/>
       <c r="I16" s="42"/>
       <c r="J16" s="42">
         <v>27</v>
@@ -7399,10 +7399,10 @@
       <c r="M16" s="42"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="70"/>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
+      <c r="A17" s="85"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
       <c r="I17" s="42"/>
       <c r="J17" s="42">
         <v>29</v>
@@ -7607,26 +7607,26 @@
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:13" ht="16" customHeight="1">
-      <c r="A29" s="71" t="s">
+      <c r="A29" s="86" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="71"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="86"/>
+      <c r="D29" s="86"/>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:13">
-      <c r="A30" s="72"/>
-      <c r="B30" s="72"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
+      <c r="A30" s="87"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="87"/>
+      <c r="D30" s="87"/>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="73"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
+      <c r="A31" s="88"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="88"/>
+      <c r="D31" s="88"/>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="34" t="s">
@@ -7735,7 +7735,7 @@
   <dimension ref="A1:U108"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:U8"/>
+      <selection activeCell="M2" sqref="M2:U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7760,97 +7760,97 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="6"/>
-      <c r="M2" s="67" t="s">
+      <c r="M2" s="82" t="s">
         <v>119</v>
       </c>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="67"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="82"/>
     </row>
     <row r="3" spans="1:21" ht="16" customHeight="1">
       <c r="B3" s="6"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
     </row>
     <row r="4" spans="1:21" ht="16" customHeight="1">
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="82"/>
+      <c r="T4" s="82"/>
+      <c r="U4" s="82"/>
     </row>
     <row r="5" spans="1:21" ht="16" customHeight="1">
-      <c r="M5" s="67"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="67"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="67"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="82"/>
+      <c r="S5" s="82"/>
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="S6" s="82"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="82"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="M7" s="67"/>
-      <c r="N7" s="67"/>
-      <c r="O7" s="67"/>
-      <c r="P7" s="67"/>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="67"/>
-      <c r="S7" s="67"/>
-      <c r="T7" s="67"/>
-      <c r="U7" s="67"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
+      <c r="P7" s="82"/>
+      <c r="Q7" s="82"/>
+      <c r="R7" s="82"/>
+      <c r="S7" s="82"/>
+      <c r="T7" s="82"/>
+      <c r="U7" s="82"/>
     </row>
     <row r="8" spans="1:21" ht="16" customHeight="1">
       <c r="B8" s="6"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="67"/>
-      <c r="P8" s="67"/>
-      <c r="Q8" s="67"/>
-      <c r="R8" s="67"/>
-      <c r="S8" s="67"/>
-      <c r="T8" s="67"/>
-      <c r="U8" s="67"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="82"/>
+      <c r="P8" s="82"/>
+      <c r="Q8" s="82"/>
+      <c r="R8" s="82"/>
+      <c r="S8" s="82"/>
+      <c r="T8" s="82"/>
+      <c r="U8" s="82"/>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
       <c r="M9" s="52" t="s">
         <v>107</v>
       </c>
@@ -7880,14 +7880,14 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="16" customHeight="1">
-      <c r="A10" s="64"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
       <c r="M10" s="42" t="s">
         <v>106</v>
       </c>
@@ -7903,14 +7903,14 @@
       <c r="U10" s="44"/>
     </row>
     <row r="11" spans="1:21" ht="16" customHeight="1">
-      <c r="A11" s="64"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
       <c r="M11" s="42"/>
       <c r="N11" s="44">
         <v>27</v>
@@ -7938,14 +7938,14 @@
       </c>
     </row>
     <row r="12" spans="1:21" ht="16" customHeight="1">
-      <c r="A12" s="74"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
+      <c r="A12" s="89"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
       <c r="M12" s="42"/>
       <c r="N12" s="44">
         <v>29</v>
@@ -8330,16 +8330,16 @@
       </c>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="78"/>
       <c r="M22" s="42"/>
       <c r="N22" s="44">
         <v>29</v>
@@ -8367,14 +8367,14 @@
       </c>
     </row>
     <row r="23" spans="1:21">
-      <c r="A23" s="64"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
+      <c r="A23" s="79"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
       <c r="M23" s="42"/>
       <c r="N23" s="43" t="s">
         <v>116</v>
@@ -8388,14 +8388,14 @@
       <c r="U23" s="44"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="64"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="64"/>
+      <c r="A24" s="79"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
       <c r="M24" s="42"/>
       <c r="N24" s="44">
         <v>27</v>
@@ -8423,14 +8423,14 @@
       </c>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="74"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="74"/>
+      <c r="A25" s="89"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="89"/>
       <c r="M25" s="42"/>
       <c r="N25" s="44">
         <v>27</v>
@@ -8900,46 +8900,46 @@
       </c>
     </row>
     <row r="39" spans="1:21">
-      <c r="A39" s="63" t="s">
+      <c r="A39" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="63"/>
-      <c r="C39" s="63"/>
-      <c r="D39" s="63"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="63"/>
-      <c r="G39" s="63"/>
-      <c r="H39" s="63"/>
+      <c r="B39" s="78"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="78"/>
+      <c r="H39" s="78"/>
     </row>
     <row r="40" spans="1:21">
-      <c r="A40" s="64"/>
-      <c r="B40" s="64"/>
-      <c r="C40" s="64"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="64"/>
-      <c r="F40" s="64"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="64"/>
+      <c r="A40" s="79"/>
+      <c r="B40" s="79"/>
+      <c r="C40" s="79"/>
+      <c r="D40" s="79"/>
+      <c r="E40" s="79"/>
+      <c r="F40" s="79"/>
+      <c r="G40" s="79"/>
+      <c r="H40" s="79"/>
     </row>
     <row r="41" spans="1:21">
-      <c r="A41" s="64"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="64"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="64"/>
-      <c r="F41" s="64"/>
-      <c r="G41" s="64"/>
-      <c r="H41" s="64"/>
+      <c r="A41" s="79"/>
+      <c r="B41" s="79"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="79"/>
+      <c r="E41" s="79"/>
+      <c r="F41" s="79"/>
+      <c r="G41" s="79"/>
+      <c r="H41" s="79"/>
     </row>
     <row r="42" spans="1:21">
-      <c r="A42" s="74"/>
-      <c r="B42" s="74"/>
-      <c r="C42" s="74"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="74"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="74"/>
+      <c r="A42" s="89"/>
+      <c r="B42" s="89"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="89"/>
+      <c r="E42" s="89"/>
+      <c r="F42" s="89"/>
+      <c r="G42" s="89"/>
+      <c r="H42" s="89"/>
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="9" t="s">
@@ -9144,46 +9144,46 @@
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="63" t="s">
+      <c r="A68" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="B68" s="63"/>
-      <c r="C68" s="63"/>
-      <c r="D68" s="63"/>
-      <c r="E68" s="63"/>
-      <c r="F68" s="63"/>
-      <c r="G68" s="63"/>
-      <c r="H68" s="63"/>
+      <c r="B68" s="78"/>
+      <c r="C68" s="78"/>
+      <c r="D68" s="78"/>
+      <c r="E68" s="78"/>
+      <c r="F68" s="78"/>
+      <c r="G68" s="78"/>
+      <c r="H68" s="78"/>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="64"/>
-      <c r="B69" s="64"/>
-      <c r="C69" s="64"/>
-      <c r="D69" s="64"/>
-      <c r="E69" s="64"/>
-      <c r="F69" s="64"/>
-      <c r="G69" s="64"/>
-      <c r="H69" s="64"/>
+      <c r="A69" s="79"/>
+      <c r="B69" s="79"/>
+      <c r="C69" s="79"/>
+      <c r="D69" s="79"/>
+      <c r="E69" s="79"/>
+      <c r="F69" s="79"/>
+      <c r="G69" s="79"/>
+      <c r="H69" s="79"/>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="64"/>
-      <c r="B70" s="64"/>
-      <c r="C70" s="64"/>
-      <c r="D70" s="64"/>
-      <c r="E70" s="64"/>
-      <c r="F70" s="64"/>
-      <c r="G70" s="64"/>
-      <c r="H70" s="64"/>
+      <c r="A70" s="79"/>
+      <c r="B70" s="79"/>
+      <c r="C70" s="79"/>
+      <c r="D70" s="79"/>
+      <c r="E70" s="79"/>
+      <c r="F70" s="79"/>
+      <c r="G70" s="79"/>
+      <c r="H70" s="79"/>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="74"/>
-      <c r="B71" s="74"/>
-      <c r="C71" s="74"/>
-      <c r="D71" s="74"/>
-      <c r="E71" s="74"/>
-      <c r="F71" s="74"/>
-      <c r="G71" s="74"/>
-      <c r="H71" s="74"/>
+      <c r="A71" s="89"/>
+      <c r="B71" s="89"/>
+      <c r="C71" s="89"/>
+      <c r="D71" s="89"/>
+      <c r="E71" s="89"/>
+      <c r="F71" s="89"/>
+      <c r="G71" s="89"/>
+      <c r="H71" s="89"/>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="9" t="s">
@@ -9340,46 +9340,46 @@
       </c>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="63" t="s">
+      <c r="A81" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="B81" s="63"/>
-      <c r="C81" s="63"/>
-      <c r="D81" s="63"/>
-      <c r="E81" s="63"/>
-      <c r="F81" s="63"/>
-      <c r="G81" s="63"/>
-      <c r="H81" s="63"/>
+      <c r="B81" s="78"/>
+      <c r="C81" s="78"/>
+      <c r="D81" s="78"/>
+      <c r="E81" s="78"/>
+      <c r="F81" s="78"/>
+      <c r="G81" s="78"/>
+      <c r="H81" s="78"/>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="64"/>
-      <c r="B82" s="64"/>
-      <c r="C82" s="64"/>
-      <c r="D82" s="64"/>
-      <c r="E82" s="64"/>
-      <c r="F82" s="64"/>
-      <c r="G82" s="64"/>
-      <c r="H82" s="64"/>
+      <c r="A82" s="79"/>
+      <c r="B82" s="79"/>
+      <c r="C82" s="79"/>
+      <c r="D82" s="79"/>
+      <c r="E82" s="79"/>
+      <c r="F82" s="79"/>
+      <c r="G82" s="79"/>
+      <c r="H82" s="79"/>
     </row>
     <row r="83" spans="1:8">
-      <c r="A83" s="64"/>
-      <c r="B83" s="64"/>
-      <c r="C83" s="64"/>
-      <c r="D83" s="64"/>
-      <c r="E83" s="64"/>
-      <c r="F83" s="64"/>
-      <c r="G83" s="64"/>
-      <c r="H83" s="64"/>
+      <c r="A83" s="79"/>
+      <c r="B83" s="79"/>
+      <c r="C83" s="79"/>
+      <c r="D83" s="79"/>
+      <c r="E83" s="79"/>
+      <c r="F83" s="79"/>
+      <c r="G83" s="79"/>
+      <c r="H83" s="79"/>
     </row>
     <row r="84" spans="1:8">
-      <c r="A84" s="74"/>
-      <c r="B84" s="74"/>
-      <c r="C84" s="74"/>
-      <c r="D84" s="74"/>
-      <c r="E84" s="74"/>
-      <c r="F84" s="74"/>
-      <c r="G84" s="74"/>
-      <c r="H84" s="74"/>
+      <c r="A84" s="89"/>
+      <c r="B84" s="89"/>
+      <c r="C84" s="89"/>
+      <c r="D84" s="89"/>
+      <c r="E84" s="89"/>
+      <c r="F84" s="89"/>
+      <c r="G84" s="89"/>
+      <c r="H84" s="89"/>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="9" t="s">
@@ -9632,46 +9632,46 @@
       </c>
     </row>
     <row r="98" spans="1:8">
-      <c r="A98" s="63" t="s">
+      <c r="A98" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="B98" s="63"/>
-      <c r="C98" s="63"/>
-      <c r="D98" s="63"/>
-      <c r="E98" s="63"/>
-      <c r="F98" s="63"/>
-      <c r="G98" s="63"/>
-      <c r="H98" s="63"/>
+      <c r="B98" s="78"/>
+      <c r="C98" s="78"/>
+      <c r="D98" s="78"/>
+      <c r="E98" s="78"/>
+      <c r="F98" s="78"/>
+      <c r="G98" s="78"/>
+      <c r="H98" s="78"/>
     </row>
     <row r="99" spans="1:8">
-      <c r="A99" s="64"/>
-      <c r="B99" s="64"/>
-      <c r="C99" s="64"/>
-      <c r="D99" s="64"/>
-      <c r="E99" s="64"/>
-      <c r="F99" s="64"/>
-      <c r="G99" s="64"/>
-      <c r="H99" s="64"/>
+      <c r="A99" s="79"/>
+      <c r="B99" s="79"/>
+      <c r="C99" s="79"/>
+      <c r="D99" s="79"/>
+      <c r="E99" s="79"/>
+      <c r="F99" s="79"/>
+      <c r="G99" s="79"/>
+      <c r="H99" s="79"/>
     </row>
     <row r="100" spans="1:8">
-      <c r="A100" s="64"/>
-      <c r="B100" s="64"/>
-      <c r="C100" s="64"/>
-      <c r="D100" s="64"/>
-      <c r="E100" s="64"/>
-      <c r="F100" s="64"/>
-      <c r="G100" s="64"/>
-      <c r="H100" s="64"/>
+      <c r="A100" s="79"/>
+      <c r="B100" s="79"/>
+      <c r="C100" s="79"/>
+      <c r="D100" s="79"/>
+      <c r="E100" s="79"/>
+      <c r="F100" s="79"/>
+      <c r="G100" s="79"/>
+      <c r="H100" s="79"/>
     </row>
     <row r="101" spans="1:8">
-      <c r="A101" s="74"/>
-      <c r="B101" s="74"/>
-      <c r="C101" s="74"/>
-      <c r="D101" s="74"/>
-      <c r="E101" s="74"/>
-      <c r="F101" s="74"/>
-      <c r="G101" s="74"/>
-      <c r="H101" s="74"/>
+      <c r="A101" s="89"/>
+      <c r="B101" s="89"/>
+      <c r="C101" s="89"/>
+      <c r="D101" s="89"/>
+      <c r="E101" s="89"/>
+      <c r="F101" s="89"/>
+      <c r="G101" s="89"/>
+      <c r="H101" s="89"/>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" s="9" t="s">
@@ -9855,7 +9855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7D0838-DBF6-D748-98D7-9545D778A035}">
   <dimension ref="C6:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -9876,27 +9876,27 @@
   </cols>
   <sheetData>
     <row r="6" spans="3:15">
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
     </row>
     <row r="7" spans="3:15" ht="16" customHeight="1">
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
     </row>
     <row r="8" spans="3:15">
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
     </row>
     <row r="9" spans="3:15" ht="17">
       <c r="C9" s="21" t="s">
@@ -10462,24 +10462,24 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:8">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="10" t="s">
@@ -10645,24 +10645,24 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:9" ht="16" customHeight="1">
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="92" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
     </row>
     <row r="6" spans="3:9">
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="93"/>
+      <c r="H6" s="93"/>
+      <c r="I6" s="93"/>
     </row>
     <row r="7" spans="3:9">
       <c r="C7" s="23" t="s">
@@ -10849,24 +10849,24 @@
       </c>
     </row>
     <row r="17" spans="3:9">
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
     </row>
     <row r="18" spans="3:9">
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
     </row>
     <row r="19" spans="3:9">
       <c r="C19" s="10" t="s">
@@ -11033,24 +11033,24 @@
   </cols>
   <sheetData>
     <row r="8" spans="3:9">
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="92" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="92"/>
     </row>
     <row r="9" spans="3:9">
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="93"/>
     </row>
     <row r="10" spans="3:9">
       <c r="C10" s="23" t="s">
@@ -11259,24 +11259,24 @@
   </cols>
   <sheetData>
     <row r="6" spans="3:9">
-      <c r="C6" s="77" t="s">
+      <c r="C6" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
     </row>
     <row r="7" spans="3:9">
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
     </row>
     <row r="8" spans="3:9">
       <c r="C8" s="23" t="s">
@@ -11478,8 +11478,8 @@
   </sheetPr>
   <dimension ref="C1:U42"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:U7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:U41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11495,82 +11495,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:21" ht="16" customHeight="1">
-      <c r="N1" s="67" t="s">
+      <c r="N1" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
     </row>
     <row r="2" spans="3:21">
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="67"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="82"/>
     </row>
     <row r="3" spans="3:21">
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
     </row>
     <row r="4" spans="3:21">
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="82"/>
+      <c r="T4" s="82"/>
+      <c r="U4" s="82"/>
     </row>
     <row r="5" spans="3:21">
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="92" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="67"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="67"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="82"/>
+      <c r="S5" s="82"/>
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
     </row>
     <row r="6" spans="3:21">
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="93"/>
+      <c r="H6" s="93"/>
+      <c r="I6" s="93"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="S6" s="82"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="82"/>
     </row>
     <row r="7" spans="3:21">
       <c r="C7" s="23" t="s">
@@ -11594,14 +11594,14 @@
       <c r="I7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="N7" s="67"/>
-      <c r="O7" s="67"/>
-      <c r="P7" s="67"/>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="67"/>
-      <c r="S7" s="67"/>
-      <c r="T7" s="67"/>
-      <c r="U7" s="67"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
+      <c r="P7" s="82"/>
+      <c r="Q7" s="82"/>
+      <c r="R7" s="82"/>
+      <c r="S7" s="82"/>
+      <c r="T7" s="82"/>
+      <c r="U7" s="82"/>
     </row>
     <row r="8" spans="3:21">
       <c r="C8" s="25" t="s">
@@ -11974,15 +11974,15 @@
       </c>
     </row>
     <row r="17" spans="3:21">
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
       <c r="N17" s="45"/>
       <c r="O17" s="55" t="s">
         <v>96</v>
@@ -12007,13 +12007,13 @@
       </c>
     </row>
     <row r="18" spans="3:21">
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
       <c r="N18" s="45"/>
       <c r="O18" s="55" t="s">
         <v>95</v>
@@ -12334,15 +12334,15 @@
       </c>
     </row>
     <row r="26" spans="3:21">
-      <c r="C26" s="77" t="s">
+      <c r="C26" s="92" t="s">
         <v>92</v>
       </c>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="77"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="92"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="92"/>
+      <c r="I26" s="92"/>
       <c r="N26" s="45"/>
       <c r="O26" s="55" t="s">
         <v>101</v>
@@ -12367,13 +12367,13 @@
       </c>
     </row>
     <row r="27" spans="3:21">
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
-      <c r="I27" s="78"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="93"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="93"/>
       <c r="N27" s="45"/>
       <c r="O27" s="55" t="s">
         <v>102</v>

</xml_diff>